<commit_message>
Remove data connection in excel spreadsheet
</commit_message>
<xml_diff>
--- a/random_forest_gridsearch.xlsx
+++ b/random_forest_gridsearch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="840" yWindow="440" windowWidth="27940" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="440" windowWidth="27940" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="gridsearch_accuracy_test" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" " comma="1" semicolon="1">
+  <connection id="1" name="gridsearch_accuracy_test" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" " comma="1" semicolon="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -43,8 +43,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="gridsearch_accuracy_test1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" " comma="1" semicolon="1">
+  <connection id="2" name="gridsearch_accuracy_test1" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" " comma="1" semicolon="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -54,8 +54,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="gridsearch_accuracy_train" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" " tab="0" semicolon="1">
+  <connection id="3" name="gridsearch_accuracy_train" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" " tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -252,12 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -265,23 +259,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -302,18 +284,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -338,7 +338,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -607,7 +607,7 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,462 +620,462 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="29" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="32"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C3" s="32">
+      <c r="C3" s="23">
         <v>2</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="24">
         <v>4</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="24">
         <v>8</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="24">
         <v>16</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="24">
         <v>32</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="24">
         <v>64</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="24">
         <v>128</v>
       </c>
-      <c r="J3" s="34">
+      <c r="J3" s="25">
         <v>256</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="32">
+      <c r="K3" s="6"/>
+      <c r="L3" s="23">
         <v>2</v>
       </c>
-      <c r="M3" s="33">
+      <c r="M3" s="24">
         <v>4</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3" s="24">
         <v>8</v>
       </c>
-      <c r="O3" s="33">
+      <c r="O3" s="24">
         <v>16</v>
       </c>
-      <c r="P3" s="33">
+      <c r="P3" s="24">
         <v>32</v>
       </c>
-      <c r="Q3" s="33">
+      <c r="Q3" s="24">
         <v>64</v>
       </c>
-      <c r="R3" s="33">
+      <c r="R3" s="24">
         <v>128</v>
       </c>
-      <c r="S3" s="34">
+      <c r="S3" s="25">
         <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="10">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="8">
         <v>0.85303333333333298</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="8">
         <v>0.86468333333333303</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>0.86431666666666596</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="9">
         <v>0.86809999999999898</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="10">
+      <c r="K4" s="8"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="8">
         <v>0.60880000000000001</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="8">
         <v>0.63260000000000005</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="8">
         <v>0.633099999999999</v>
       </c>
-      <c r="S4" s="11">
+      <c r="S4" s="9">
         <v>0.64539999999999897</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="34"/>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="10">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="8">
         <v>0.85394999999999899</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>0.86486666666666601</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>0.86548333333333305</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="9">
         <v>0.86916666666666598</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="10">
+      <c r="K5" s="8"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="8">
         <v>0.60140000000000005</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="8">
         <v>0.62539999999999896</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="8">
         <v>0.63380000000000003</v>
       </c>
-      <c r="S5" s="11">
+      <c r="S5" s="9">
         <v>0.637099999999999</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="34"/>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="10">
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="8">
         <v>0.97594999999999898</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="8">
         <v>0.97423333333333295</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>0.97135000000000005</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <v>0.96968333333333301</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="10">
+      <c r="K6" s="8"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="8">
         <v>0.72030000000000005</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="8">
         <v>0.72250000000000003</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="8">
         <v>0.72250000000000003</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S6" s="9">
         <v>0.71379999999999899</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="34"/>
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="10">
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="8">
         <v>0.99546666666666594</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="8">
         <v>0.99460000000000004</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="8">
         <v>0.99273333333333302</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="9">
         <v>0.99099999999999899</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="10">
+      <c r="K7" s="8"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="8">
         <v>0.7671</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="8">
         <v>0.76559999999999895</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="8">
         <v>0.75509999999999899</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="9">
         <v>0.74829999999999897</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="34"/>
       <c r="B8">
         <v>20</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="10">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="8">
         <v>0.99944999999999895</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="8">
         <v>0.99928333333333297</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="8">
         <v>0.99861666666666604</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="9">
         <v>0.99804999999999899</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="10">
+      <c r="K8" s="8"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="8">
         <v>0.79859999999999898</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="8">
         <v>0.78459999999999896</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="8">
         <v>0.77629999999999899</v>
       </c>
-      <c r="S8" s="11">
+      <c r="S8" s="9">
         <v>0.76370000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="34"/>
       <c r="B9">
         <v>50</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="26">
         <v>0.999966666666666</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="10">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="8">
         <v>0.999966666666666</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <v>0.99990000000000001</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="9">
         <v>0.99978333333333302</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="20">
+      <c r="K9" s="8"/>
+      <c r="L9" s="14">
         <v>0.83620000000000005</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="15">
         <v>0.83309999999999895</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="15">
         <v>0.83640000000000003</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="15">
         <v>0.82730000000000004</v>
       </c>
-      <c r="P9" s="21">
+      <c r="P9" s="15">
         <v>0.81630000000000003</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="8">
         <v>0.80059999999999898</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="8">
         <v>0.78890000000000005</v>
       </c>
-      <c r="S9" s="11">
+      <c r="S9" s="9">
         <v>0.77159999999999895</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="34"/>
       <c r="B10">
         <v>100</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="20">
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="14">
         <v>0.84589999999999899</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="15">
         <v>0.84750000000000003</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="15">
         <v>0.84350000000000003</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="15">
         <v>0.83399999999999896</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="15">
         <v>0.82350000000000001</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="9"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="34"/>
       <c r="B11">
         <v>200</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="20">
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="14">
         <v>0.85550000000000004</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="15">
         <v>0.85360000000000003</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="15">
         <v>0.84640000000000004</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="15">
         <v>0.83720000000000006</v>
       </c>
-      <c r="P11" s="21">
+      <c r="P11" s="15">
         <v>0.82720000000000005</v>
       </c>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="9"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="34"/>
       <c r="B12">
         <v>1000</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="22">
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="16">
         <v>0.86209999999999898</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="17">
         <v>0.85840000000000005</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="17">
         <v>0.85140000000000005</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O12" s="17">
         <v>0.84079999999999899</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P12" s="17">
         <v>0.82750000000000001</v>
       </c>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="25"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="19"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
+      <c r="A13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
@@ -1134,32 +1134,32 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>